<commit_message>
In advanced inputs excel, now the industry does not have to be created
</commit_message>
<xml_diff>
--- a/dist/wiat_template.xlsx
+++ b/dist/wiat_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\PhpstormProjects\wiat_front\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6878C23C-4916-4F16-ABC5-AC0E4B57A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FD0B81-4E98-4FB3-94AB-243FB816E9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{A14C6850-7486-4D49-86A3-639AED911610}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{A14C6850-7486-4D49-86A3-639AED911610}"/>
   </bookViews>
   <sheets>
     <sheet name="INDUSTRY" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="187">
   <si>
     <t>Assessment name</t>
   </si>
@@ -734,6 +734,22 @@
 2 --&gt; Modeled (data that you have extracted from a scientific model. It would typically be more accurate than estimated data, and less accurate than measured data)
 3 --&gt; User data (measured)</t>
     </r>
+  </si>
+  <si>
+    <t>Latidude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Suppliers</t>
+  </si>
+  <si>
+    <t>Add as many suppliers (Name, Latitude, 
+Longitude) as needed to the right (ignore level of certainty)</t>
+  </si>
+  <si>
+    <t>INDUSTRY DEFINITION</t>
   </si>
 </sst>
 </file>
@@ -1087,6 +1103,21 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1096,31 +1127,18 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Énfasis1" xfId="3" builtinId="30"/>
@@ -1441,10 +1459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D97F1C-3547-4525-AD16-36CC009A61DF}">
-  <dimension ref="A2:I32"/>
+  <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1452,7 +1470,7 @@
     <col min="1" max="1" width="20.453125" customWidth="1"/>
     <col min="2" max="2" width="18.90625" customWidth="1"/>
     <col min="3" max="3" width="43.1796875" customWidth="1"/>
-    <col min="4" max="4" width="31.54296875" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" customWidth="1"/>
     <col min="5" max="5" width="18.453125" customWidth="1"/>
     <col min="6" max="6" width="17.36328125" customWidth="1"/>
     <col min="9" max="9" width="48.90625" customWidth="1"/>
@@ -1473,7 +1491,9 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="36"/>
+      <c r="A3" s="39" t="s">
+        <v>186</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1496,224 +1516,259 @@
       <c r="E4" s="4"/>
       <c r="F4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="72.5">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="36"/>
+      <c r="B5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="36"/>
+      <c r="B6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" ht="54.5" customHeight="1">
+      <c r="A7" s="36"/>
+      <c r="B7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="55" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:9" ht="72.5">
+      <c r="A8" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B8" s="28" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="I5" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="53.5" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="4"/>
-      <c r="I6" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="131" thickBot="1">
-      <c r="A7" s="37"/>
-      <c r="B7" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="4"/>
-      <c r="I7" s="34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="131" thickBot="1">
-      <c r="A8" s="37"/>
-      <c r="B8" s="28" t="s">
-        <v>50</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>51</v>
+      <c r="D8" s="31" t="s">
+        <v>174</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="17"/>
-      <c r="I8" s="35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="58">
+      <c r="F8" s="4"/>
+      <c r="I8" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="53.5" customHeight="1">
       <c r="A9" s="37"/>
       <c r="B9" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="I9" s="55"/>
-    </row>
-    <row r="10" spans="1:9" ht="72.5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="4"/>
+      <c r="I9" s="33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="131" thickBot="1">
       <c r="A10" s="37"/>
       <c r="B10" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:9" ht="72.5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="4"/>
+      <c r="I10" s="34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="131" thickBot="1">
       <c r="A11" s="37"/>
       <c r="B11" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="20"/>
-    </row>
-    <row r="12" spans="1:9" ht="29" customHeight="1">
+        <v>50</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="17"/>
+      <c r="I11" s="35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="58">
       <c r="A12" s="37"/>
       <c r="B12" s="28" t="s">
-        <v>159</v>
+        <v>52</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>17</v>
+        <v>173</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="188.5">
+    <row r="13" spans="1:9" ht="72.5">
       <c r="A13" s="37"/>
       <c r="B13" s="28" t="s">
-        <v>160</v>
+        <v>7</v>
       </c>
       <c r="C13" s="24"/>
-      <c r="D13" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="D13" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="58">
+    <row r="14" spans="1:9" ht="72.5">
       <c r="A14" s="37"/>
       <c r="B14" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>54</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C14" s="24"/>
       <c r="D14" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:9" ht="72.5">
+        <v>175</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" ht="29" customHeight="1">
       <c r="A15" s="37"/>
       <c r="B15" s="28" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C15" s="24"/>
-      <c r="D15" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="87">
+      <c r="D15" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" ht="188.5">
       <c r="A16" s="37"/>
-      <c r="B16" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>166</v>
+      <c r="B16" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="18"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:8" ht="58">
       <c r="A17" s="37"/>
-      <c r="B17" s="23" t="s">
-        <v>60</v>
+      <c r="B17" s="28" t="s">
+        <v>161</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="25"/>
+        <v>54</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>176</v>
+      </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="1:8" ht="87">
-      <c r="A18" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>166</v>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" ht="72.5">
+      <c r="A18" s="37"/>
+      <c r="B18" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="H19" s="18"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="B32" s="18"/>
+    </row>
+    <row r="19" spans="1:8" ht="87">
+      <c r="A19" s="37"/>
+      <c r="B19" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" ht="58">
+      <c r="A20" s="37"/>
+      <c r="B20" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" ht="87">
+      <c r="A21" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="H22" s="18"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A17"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1724,13 +1779,13 @@
           <x14:formula1>
             <xm:f>Hoja5!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E9:E11</xm:sqref>
+          <xm:sqref>E12:E14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{87702C7D-FEA7-4548-AAEE-A11AD64184A6}">
           <x14:formula1>
             <xm:f>Hoja5!$F$3:$F$27</xm:f>
           </x14:formula1>
-          <xm:sqref>E12</xm:sqref>
+          <xm:sqref>E15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1742,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3699978A-1E09-4AD2-9D2E-EA46A24DCBD2}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -3005,7 +3060,7 @@
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" ht="29">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B18" s="23" t="s">
@@ -3021,7 +3076,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="14.5" customHeight="1">
-      <c r="A19" s="51"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="23" t="s">
         <v>95</v>
       </c>
@@ -3033,7 +3088,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="43.5">
-      <c r="A20" s="51"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="23" t="s">
         <v>97</v>
       </c>
@@ -3047,7 +3102,7 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="51"/>
+      <c r="A21" s="52"/>
       <c r="B21" s="23" t="s">
         <v>99</v>
       </c>
@@ -3059,7 +3114,7 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="51"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="23" t="s">
         <v>100</v>
       </c>
@@ -3071,7 +3126,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="51"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="23" t="s">
         <v>101</v>
       </c>
@@ -3083,7 +3138,7 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="51"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="23" t="s">
         <v>102</v>
       </c>
@@ -3097,7 +3152,7 @@
       <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="52"/>
+      <c r="A25" s="45"/>
       <c r="B25" s="23" t="s">
         <v>103</v>
       </c>
@@ -3109,7 +3164,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="49" t="s">
         <v>150</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -3125,7 +3180,7 @@
       <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:7" ht="14.5" customHeight="1">
-      <c r="A27" s="46"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="1" t="s">
         <v>105</v>
       </c>
@@ -3137,7 +3192,7 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="46" t="s">
         <v>151</v>
       </c>
       <c r="B28" s="23" t="s">
@@ -3151,7 +3206,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="48"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="23" t="s">
         <v>107</v>
       </c>
@@ -3163,7 +3218,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="29">
-      <c r="A30" s="48"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="23" t="s">
         <v>109</v>
       </c>
@@ -3175,7 +3230,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="48"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="23" t="s">
         <v>110</v>
       </c>
@@ -3187,7 +3242,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="49"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="23" t="s">
         <v>111</v>
       </c>
@@ -3199,7 +3254,7 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="49" t="s">
         <v>152</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -3215,7 +3270,7 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="29">
-      <c r="A34" s="45"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="1" t="s">
         <v>114</v>
       </c>
@@ -3229,7 +3284,7 @@
       <c r="F34" s="20"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="45"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="1" t="s">
         <v>115</v>
       </c>
@@ -3241,7 +3296,7 @@
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="29">
-      <c r="A36" s="45"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="1" t="s">
         <v>116</v>
       </c>
@@ -3253,7 +3308,7 @@
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="45"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="1" t="s">
         <v>117</v>
       </c>
@@ -3265,7 +3320,7 @@
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="45"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="1" t="s">
         <v>118</v>
       </c>
@@ -3277,7 +3332,7 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="29">
-      <c r="A39" s="45"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="1" t="s">
         <v>119</v>
       </c>
@@ -3289,7 +3344,7 @@
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="46"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="1" t="s">
         <v>121</v>
       </c>
@@ -3301,7 +3356,7 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="46" t="s">
         <v>153</v>
       </c>
       <c r="B41" s="26" t="s">
@@ -3315,7 +3370,7 @@
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="29">
-      <c r="A42" s="48"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="23" t="s">
         <v>124</v>
       </c>
@@ -3329,7 +3384,7 @@
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="48"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="26" t="s">
         <v>128</v>
       </c>
@@ -3341,7 +3396,7 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="49"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="26" t="s">
         <v>127</v>
       </c>
@@ -3553,7 +3608,7 @@
       <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" ht="29">
-      <c r="A61" s="50" t="s">
+      <c r="A61" s="44" t="s">
         <v>157</v>
       </c>
       <c r="B61" s="23" t="s">
@@ -3569,7 +3624,7 @@
       <c r="F61" s="20"/>
     </row>
     <row r="62" spans="1:6" ht="14.5" customHeight="1">
-      <c r="A62" s="52"/>
+      <c r="A62" s="45"/>
       <c r="B62" s="23" t="s">
         <v>105</v>
       </c>
@@ -3585,17 +3640,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A50:A58"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A41:A44"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A33:A40"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A18:A25"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A41:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>